<commit_message>
minor changes. starting with second run per month spaced start date
</commit_message>
<xml_diff>
--- a/all_times_14_flat/Runs_reports_static_lot/None_all_times_14_flat_static_pnl_growth_report_TR1500_DD1500_SZ1_TDDTrue_monthly.xlsx
+++ b/all_times_14_flat/Runs_reports_static_lot/None_all_times_14_flat_static_pnl_growth_report_TR1500_DD1500_SZ1_TDDTrue_monthly.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vova deduskin lap\PycharmProjects\1500_count\all_times_14_flat\Runs_reports_static_lot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liikurserv\PycharmProjects\1500_count\all_times_14_flat\Runs_reports_static_lot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5643774-FA04-4B4F-A1EB-F7B3F0A9533B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966185FC-ECFB-41FB-8EE8-1F88C892DDE9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,13 +501,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -534,10 +547,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -546,11 +560,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -886,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -1359,58 +1384,62 @@
         <f>SUBTOTAL(3,A2:A9)</f>
         <v>8</v>
       </c>
+      <c r="B10">
+        <f>SUBTOTAL(3,B2:B9)</f>
+        <v>7</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="P10" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:17" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:17" s="7" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>43832</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>48</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>1500</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
         <v>43899</v>
       </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="I11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="7">
         <v>100</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="7">
         <v>48</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="7">
         <v>2</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="7">
         <v>80</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="7">
         <v>2020</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="7">
         <v>840</v>
       </c>
     </row>
@@ -1969,6 +1998,10 @@
         <f>SUBTOTAL(3,A11:A22)</f>
         <v>12</v>
       </c>
+      <c r="B23">
+        <f>SUBTOTAL(3,B11:B22)</f>
+        <v>8</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="P23" s="3" t="s">
         <v>144</v>
@@ -2579,6 +2612,10 @@
         <f>SUBTOTAL(3,A24:A35)</f>
         <v>12</v>
       </c>
+      <c r="B36">
+        <f>SUBTOTAL(3,B24:B35)</f>
+        <v>8</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="P36" s="3" t="s">
         <v>145</v>
@@ -3189,6 +3226,10 @@
         <f>SUBTOTAL(3,A37:A48)</f>
         <v>12</v>
       </c>
+      <c r="B49">
+        <f>SUBTOTAL(3,B37:B48)</f>
+        <v>11</v>
+      </c>
       <c r="H49" s="2"/>
       <c r="P49" s="3" t="s">
         <v>146</v>
@@ -3799,6 +3840,10 @@
         <f>SUBTOTAL(3,A50:A61)</f>
         <v>12</v>
       </c>
+      <c r="B62">
+        <f>SUBTOTAL(3,B50:B61)</f>
+        <v>7</v>
+      </c>
       <c r="H62" s="2"/>
       <c r="P62" s="3" t="s">
         <v>147</v>
@@ -4409,6 +4454,10 @@
         <f>SUBTOTAL(3,A63:A74)</f>
         <v>12</v>
       </c>
+      <c r="B75">
+        <f>SUBTOTAL(3,B63:B74)</f>
+        <v>11</v>
+      </c>
       <c r="H75" s="2"/>
       <c r="P75" s="3" t="s">
         <v>148</v>
@@ -4904,6 +4953,10 @@
         <f>SUBTOTAL(3,A76:A85)</f>
         <v>10</v>
       </c>
+      <c r="B86">
+        <f>SUBTOTAL(3,B76:B85)</f>
+        <v>6</v>
+      </c>
       <c r="P86" s="3" t="s">
         <v>149</v>
       </c>
@@ -4912,6 +4965,10 @@
       <c r="A87" s="5">
         <f>SUBTOTAL(3,A2:A85)</f>
         <v>78</v>
+      </c>
+      <c r="B87">
+        <f>SUBTOTAL(3,B2:B85)</f>
+        <v>58</v>
       </c>
       <c r="P87" s="3" t="s">
         <v>150</v>
@@ -5158,6 +5215,11 @@
       <c r="D108" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5779,7 +5841,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>